<commit_message>
update Schedule and Manual file
</commit_message>
<xml_diff>
--- a/2.スケジュール/スケジュール.xlsx
+++ b/2.スケジュール/スケジュール.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\GitHub\Rootstock_SC\2.スケジュール\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E760874-3195-4E51-8DE1-058AC89D7C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433DCD4F-AEE6-42A4-ACEA-B38FDEAD0200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-2340" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC3888E-2072-4F01-B82D-11B88CE59715}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="807">
   <si>
     <t>項目</t>
     <rPh sb="0" eb="2">
@@ -3284,6 +3284,97 @@
     </rPh>
     <rPh sb="35" eb="37">
       <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>VAT Classを調べる</t>
+    <rPh sb="10" eb="11">
+      <t>シラ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AppLauncher（7つ）</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SendMail</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>受注</t>
+  </si>
+  <si>
+    <t>出荷</t>
+  </si>
+  <si>
+    <t>生産計画・製造</t>
+  </si>
+  <si>
+    <t>調達</t>
+  </si>
+  <si>
+    <t>在庫・棚卸</t>
+  </si>
+  <si>
+    <t>マスタ</t>
+  </si>
+  <si>
+    <t>請求書</t>
+  </si>
+  <si>
+    <t>PO RecieptのUpload機能</t>
+    <rPh sb="17" eb="19">
+      <t>キノウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>QA No85と森下さんのメールを確認</t>
+    <rPh sb="8" eb="10">
+      <t>モリシタ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>・コメントと黄色い所を確認
+・サイト、在庫ロケーションIDを更新</t>
+    <rPh sb="6" eb="8">
+      <t>キイロ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>トコロ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ザイコ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>No60と同じ</t>
+    <rPh sb="5" eb="6">
+      <t>オナ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>北川さんのメールを確認
+Rootforms発注書メール自動送信_V1_0.docx</t>
+    <rPh sb="0" eb="2">
+      <t>キタガワ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>カクニン</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -3418,7 +3509,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3463,7 +3554,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3540,7 +3637,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3706,9 +3803,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3723,9 +3817,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -3745,12 +3836,6 @@
     <xf numFmtId="38" fontId="13" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3761,15 +3846,48 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="13" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="13" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3782,42 +3900,45 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="13" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="13" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3826,7 +3947,7 @@
     <cellStyle name="桁区切り" xfId="2" builtinId="6"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
     <dxf>
       <font>
         <color auto="1"/>
@@ -3852,9 +3973,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3866,12 +3990,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4211,28 +4356,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7929DC-B531-419A-8BB3-4B492C6A9455}">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="F36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H53" sqref="H53"/>
+      <selection pane="bottomRight" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="3.5" style="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.875" style="63" customWidth="1"/>
-    <col min="3" max="3" width="20.375" style="63" customWidth="1"/>
+    <col min="2" max="2" width="21.875" style="61" customWidth="1"/>
+    <col min="3" max="3" width="20.375" style="61" customWidth="1"/>
     <col min="4" max="4" width="14.125" style="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" style="64" customWidth="1"/>
-    <col min="6" max="6" width="14.125" style="64" customWidth="1"/>
-    <col min="7" max="9" width="12.375" style="64" customWidth="1"/>
-    <col min="10" max="10" width="13.625" style="65" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.625" style="65" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.625" style="65" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.625" style="65" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" style="62" customWidth="1"/>
+    <col min="6" max="6" width="14.125" style="62" customWidth="1"/>
+    <col min="7" max="9" width="12.375" style="62" customWidth="1"/>
+    <col min="10" max="10" width="13.625" style="63" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.625" style="63" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.625" style="63" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.625" style="63" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="35" style="47" customWidth="1"/>
     <col min="15" max="15" width="17.125" style="47" customWidth="1"/>
     <col min="16" max="16384" width="8.625" style="47"/>
@@ -4286,14 +4431,14 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A2" s="72">
+      <c r="A2" s="68">
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="70" t="s">
         <v>711</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="70" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="48" t="s">
@@ -4308,14 +4453,15 @@
       </c>
       <c r="H2" s="49"/>
       <c r="I2" s="51" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="J2" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K2" s="53"/>
       <c r="L2" s="52">
-        <v>45090</v>
+        <f>J2+3</f>
+        <v>45106</v>
       </c>
       <c r="M2" s="53"/>
       <c r="N2" s="54" t="s">
@@ -4324,12 +4470,12 @@
       <c r="O2" s="54"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A3" s="72">
+      <c r="A3" s="68">
         <f t="shared" ref="A3:A52" si="0">ROW()-1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
       <c r="D3" s="48" t="s">
         <v>717</v>
       </c>
@@ -4342,14 +4488,15 @@
       </c>
       <c r="H3" s="49"/>
       <c r="I3" s="51" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="J3" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K3" s="53"/>
       <c r="L3" s="52">
-        <v>45090</v>
+        <f t="shared" ref="L3:L14" si="1">J3+3</f>
+        <v>45106</v>
       </c>
       <c r="M3" s="53"/>
       <c r="N3" s="54" t="s">
@@ -4358,12 +4505,12 @@
       <c r="O3" s="54"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A4" s="72">
+      <c r="A4" s="68">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="48" t="s">
         <v>718</v>
       </c>
@@ -4375,29 +4522,30 @@
         <v>60</v>
       </c>
       <c r="H4" s="49"/>
-      <c r="I4" s="55" t="s">
-        <v>763</v>
+      <c r="I4" s="99" t="s">
+        <v>762</v>
       </c>
       <c r="J4" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K4" s="53"/>
       <c r="L4" s="52">
-        <v>45090</v>
+        <f t="shared" si="1"/>
+        <v>45106</v>
       </c>
       <c r="M4" s="53"/>
-      <c r="N4" s="56" t="s">
+      <c r="N4" s="55" t="s">
         <v>782</v>
       </c>
       <c r="O4" s="54"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A5" s="72">
+      <c r="A5" s="68">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="48" t="s">
         <v>719</v>
       </c>
@@ -4413,11 +4561,12 @@
         <v>762</v>
       </c>
       <c r="J5" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K5" s="53"/>
       <c r="L5" s="52">
-        <v>45090</v>
+        <f t="shared" si="1"/>
+        <v>45106</v>
       </c>
       <c r="M5" s="53"/>
       <c r="N5" s="54" t="s">
@@ -4426,12 +4575,12 @@
       <c r="O5" s="54"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A6" s="72">
+      <c r="A6" s="68">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="57" t="s">
+      <c r="B6" s="70"/>
+      <c r="C6" s="56" t="s">
         <v>713</v>
       </c>
       <c r="D6" s="48"/>
@@ -4447,11 +4596,12 @@
         <v>762</v>
       </c>
       <c r="J6" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K6" s="53"/>
       <c r="L6" s="52">
-        <v>45090</v>
+        <f t="shared" si="1"/>
+        <v>45106</v>
       </c>
       <c r="M6" s="53"/>
       <c r="N6" s="54" t="s">
@@ -4460,15 +4610,15 @@
       <c r="O6" s="54"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A7" s="72">
+      <c r="A7" s="68">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73" t="s">
+      <c r="B7" s="70"/>
+      <c r="C7" s="70" t="s">
         <v>715</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="57" t="s">
         <v>720</v>
       </c>
       <c r="E7" s="49">
@@ -4483,11 +4633,12 @@
         <v>762</v>
       </c>
       <c r="J7" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K7" s="52"/>
       <c r="L7" s="52">
-        <v>45090</v>
+        <f t="shared" si="1"/>
+        <v>45106</v>
       </c>
       <c r="M7" s="52"/>
       <c r="N7" s="54" t="s">
@@ -4496,13 +4647,13 @@
       <c r="O7" s="54"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A8" s="72">
+      <c r="A8" s="68">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="59" t="s">
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="58" t="s">
         <v>721</v>
       </c>
       <c r="E8" s="49">
@@ -4517,11 +4668,12 @@
         <v>762</v>
       </c>
       <c r="J8" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K8" s="52"/>
       <c r="L8" s="52">
-        <v>45090</v>
+        <f t="shared" si="1"/>
+        <v>45106</v>
       </c>
       <c r="M8" s="52"/>
       <c r="N8" s="54" t="s">
@@ -4530,15 +4682,15 @@
       <c r="O8" s="54"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A9" s="72">
+      <c r="A9" s="68">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="57" t="s">
+      <c r="B9" s="70"/>
+      <c r="C9" s="56" t="s">
         <v>714</v>
       </c>
-      <c r="D9" s="59"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="49">
         <v>100</v>
       </c>
@@ -4551,11 +4703,12 @@
         <v>762</v>
       </c>
       <c r="J9" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K9" s="52"/>
       <c r="L9" s="52">
-        <v>45090</v>
+        <f t="shared" si="1"/>
+        <v>45106</v>
       </c>
       <c r="M9" s="52"/>
       <c r="N9" s="54" t="s">
@@ -4564,12 +4717,12 @@
       <c r="O9" s="54"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A10" s="72">
+      <c r="A10" s="68">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73" t="s">
+      <c r="B10" s="70"/>
+      <c r="C10" s="70" t="s">
         <v>712</v>
       </c>
       <c r="D10" s="48" t="s">
@@ -4587,11 +4740,12 @@
         <v>762</v>
       </c>
       <c r="J10" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K10" s="52"/>
       <c r="L10" s="52">
-        <v>45090</v>
+        <f t="shared" si="1"/>
+        <v>45106</v>
       </c>
       <c r="M10" s="52"/>
       <c r="N10" s="54" t="s">
@@ -4600,13 +4754,13 @@
       <c r="O10" s="54"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A11" s="72">
+      <c r="A11" s="68">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="59" t="s">
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="58" t="s">
         <v>722</v>
       </c>
       <c r="E11" s="49">
@@ -4621,11 +4775,12 @@
         <v>762</v>
       </c>
       <c r="J11" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K11" s="52"/>
       <c r="L11" s="52">
-        <v>45090</v>
+        <f t="shared" si="1"/>
+        <v>45106</v>
       </c>
       <c r="M11" s="52"/>
       <c r="N11" s="54" t="s">
@@ -4634,13 +4789,13 @@
       <c r="O11" s="54"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A12" s="72">
+      <c r="A12" s="68">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="59" t="s">
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="58" t="s">
         <v>723</v>
       </c>
       <c r="E12" s="49">
@@ -4655,11 +4810,12 @@
         <v>762</v>
       </c>
       <c r="J12" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K12" s="52"/>
       <c r="L12" s="52">
-        <v>45090</v>
+        <f t="shared" si="1"/>
+        <v>45106</v>
       </c>
       <c r="M12" s="52"/>
       <c r="N12" s="54" t="s">
@@ -4668,12 +4824,12 @@
       <c r="O12" s="54"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A13" s="72">
+      <c r="A13" s="68">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73" t="s">
+      <c r="B13" s="70"/>
+      <c r="C13" s="70" t="s">
         <v>724</v>
       </c>
       <c r="D13" s="48" t="s">
@@ -4691,11 +4847,12 @@
         <v>762</v>
       </c>
       <c r="J13" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K13" s="52"/>
       <c r="L13" s="52">
-        <v>45090</v>
+        <f t="shared" si="1"/>
+        <v>45106</v>
       </c>
       <c r="M13" s="52"/>
       <c r="N13" s="54" t="s">
@@ -4704,12 +4861,12 @@
       <c r="O13" s="54"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A14" s="72">
+      <c r="A14" s="68">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="48" t="s">
         <v>726</v>
       </c>
@@ -4725,11 +4882,12 @@
         <v>762</v>
       </c>
       <c r="J14" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K14" s="52"/>
       <c r="L14" s="52">
-        <v>45090</v>
+        <f t="shared" si="1"/>
+        <v>45106</v>
       </c>
       <c r="M14" s="52"/>
       <c r="N14" s="54" t="s">
@@ -4738,184 +4896,200 @@
       <c r="O14" s="54"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A15" s="72">
+      <c r="A15" s="68">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="70" t="s">
         <v>727</v>
       </c>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="56" t="s">
         <v>716</v>
       </c>
       <c r="D15" s="48"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
+      <c r="E15" s="71">
+        <v>100</v>
+      </c>
+      <c r="F15" s="71"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="71"/>
       <c r="I15" s="51" t="s">
         <v>762</v>
       </c>
       <c r="J15" s="52">
         <v>45079</v>
       </c>
-      <c r="K15" s="52"/>
+      <c r="K15" s="52">
+        <v>45092</v>
+      </c>
       <c r="L15" s="52">
         <v>45079</v>
       </c>
-      <c r="M15" s="52"/>
+      <c r="M15" s="52">
+        <v>45094</v>
+      </c>
       <c r="N15" s="54"/>
       <c r="O15" s="54"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A16" s="72">
+      <c r="A16" s="68">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="73"/>
-      <c r="C16" s="57" t="s">
+      <c r="B16" s="70"/>
+      <c r="C16" s="56" t="s">
         <v>729</v>
       </c>
       <c r="D16" s="48"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
+      <c r="E16" s="71">
+        <v>80</v>
+      </c>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
       <c r="I16" s="51" t="s">
         <v>762</v>
       </c>
       <c r="J16" s="52">
         <v>45082</v>
       </c>
-      <c r="K16" s="52"/>
+      <c r="K16" s="52">
+        <v>45092</v>
+      </c>
       <c r="L16" s="52">
-        <v>45082</v>
+        <v>45106</v>
       </c>
       <c r="M16" s="52"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="60"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="59"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A17" s="72">
+      <c r="A17" s="68">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="73"/>
-      <c r="C17" s="57" t="s">
+      <c r="B17" s="70"/>
+      <c r="C17" s="56" t="s">
         <v>730</v>
       </c>
       <c r="D17" s="48"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
       <c r="I17" s="51" t="s">
         <v>762</v>
       </c>
       <c r="J17" s="52">
-        <v>45082</v>
+        <v>45103</v>
       </c>
       <c r="K17" s="52"/>
       <c r="L17" s="52">
-        <v>45082</v>
+        <v>45103</v>
       </c>
       <c r="M17" s="52"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="60"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="59"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A18" s="72">
+      <c r="A18" s="68">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="57" t="s">
+      <c r="B18" s="70"/>
+      <c r="C18" s="56" t="s">
         <v>731</v>
       </c>
       <c r="D18" s="48"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
+      <c r="E18" s="71">
+        <v>100</v>
+      </c>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
       <c r="I18" s="51" t="s">
         <v>762</v>
       </c>
       <c r="J18" s="52">
         <v>45083</v>
       </c>
-      <c r="K18" s="52"/>
+      <c r="K18" s="52">
+        <v>45097</v>
+      </c>
       <c r="L18" s="52">
         <v>45083</v>
       </c>
-      <c r="M18" s="52"/>
+      <c r="M18" s="52">
+        <v>45097</v>
+      </c>
       <c r="N18" s="54"/>
       <c r="O18" s="54"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A19" s="72">
+      <c r="A19" s="68">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="57" t="s">
+      <c r="B19" s="70"/>
+      <c r="C19" s="56" t="s">
         <v>750</v>
       </c>
       <c r="D19" s="48"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="76"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
       <c r="I19" s="51" t="s">
         <v>762</v>
       </c>
       <c r="J19" s="52">
-        <v>45083</v>
+        <v>45104</v>
       </c>
       <c r="K19" s="52"/>
       <c r="L19" s="52">
-        <v>45083</v>
+        <v>45105</v>
       </c>
       <c r="M19" s="52"/>
       <c r="N19" s="54"/>
       <c r="O19" s="54"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A20" s="72">
+      <c r="A20" s="68">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="56" t="s">
         <v>728</v>
       </c>
-      <c r="C20" s="57"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="48"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="76"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
       <c r="I20" s="51" t="s">
         <v>762</v>
       </c>
       <c r="J20" s="52">
-        <v>45089</v>
+        <v>45104</v>
       </c>
       <c r="K20" s="52"/>
       <c r="L20" s="52">
-        <v>45093</v>
+        <v>45105</v>
       </c>
       <c r="M20" s="52"/>
       <c r="N20" s="54"/>
       <c r="O20" s="54"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A21" s="72">
+      <c r="A21" s="68">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="57"/>
+      <c r="C21" s="56"/>
       <c r="D21" s="48"/>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -4925,7 +5099,7 @@
         <v>762</v>
       </c>
       <c r="J21" s="52">
-        <v>45089</v>
+        <v>45103</v>
       </c>
       <c r="K21" s="52"/>
       <c r="L21" s="52">
@@ -4936,142 +5110,142 @@
       <c r="O21" s="54"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A22" s="72">
+      <c r="A22" s="68">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="89" t="s">
         <v>732</v>
       </c>
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="90" t="s">
         <v>734</v>
       </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49">
+      <c r="D22" s="91"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92">
         <v>80</v>
       </c>
-      <c r="H22" s="49"/>
-      <c r="I22" s="51" t="s">
+      <c r="H22" s="92"/>
+      <c r="I22" s="93" t="s">
         <v>762</v>
       </c>
-      <c r="J22" s="52">
+      <c r="J22" s="94">
         <v>45092</v>
       </c>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52">
+      <c r="K22" s="94"/>
+      <c r="L22" s="94">
         <v>45092</v>
       </c>
-      <c r="M22" s="52"/>
-      <c r="N22" s="54" t="s">
+      <c r="M22" s="94"/>
+      <c r="N22" s="91" t="s">
         <v>783</v>
       </c>
       <c r="O22" s="54"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A23" s="72">
+      <c r="A23" s="68">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="57" t="s">
+      <c r="B23" s="89"/>
+      <c r="C23" s="90" t="s">
         <v>735</v>
       </c>
-      <c r="D23" s="48"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49">
+      <c r="D23" s="91"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="92">
         <v>80</v>
       </c>
-      <c r="H23" s="49"/>
-      <c r="I23" s="51" t="s">
+      <c r="H23" s="92"/>
+      <c r="I23" s="93" t="s">
         <v>762</v>
       </c>
-      <c r="J23" s="52">
+      <c r="J23" s="94">
         <v>45092</v>
       </c>
-      <c r="K23" s="53"/>
-      <c r="L23" s="52">
+      <c r="K23" s="95"/>
+      <c r="L23" s="94">
         <v>45092</v>
       </c>
-      <c r="M23" s="53"/>
-      <c r="N23" s="54" t="s">
+      <c r="M23" s="95"/>
+      <c r="N23" s="91" t="s">
         <v>783</v>
       </c>
       <c r="O23" s="54"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A24" s="72">
+      <c r="A24" s="68">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="75"/>
-      <c r="C24" s="57" t="s">
+      <c r="B24" s="89"/>
+      <c r="C24" s="90" t="s">
         <v>736</v>
       </c>
-      <c r="D24" s="48"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49">
+      <c r="D24" s="91"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="92">
         <v>60</v>
       </c>
-      <c r="H24" s="49"/>
-      <c r="I24" s="51" t="s">
+      <c r="H24" s="92"/>
+      <c r="I24" s="93" t="s">
         <v>762</v>
       </c>
-      <c r="J24" s="52">
+      <c r="J24" s="94">
         <v>45092</v>
       </c>
-      <c r="K24" s="53"/>
-      <c r="L24" s="52">
+      <c r="K24" s="95"/>
+      <c r="L24" s="94">
         <v>45092</v>
       </c>
-      <c r="M24" s="53"/>
-      <c r="N24" s="54" t="s">
+      <c r="M24" s="95"/>
+      <c r="N24" s="91" t="s">
         <v>783</v>
       </c>
       <c r="O24" s="54"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A25" s="72">
+      <c r="A25" s="68">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="75"/>
-      <c r="C25" s="57" t="s">
+      <c r="B25" s="89"/>
+      <c r="C25" s="90" t="s">
         <v>733</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="51" t="s">
+      <c r="D25" s="91"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="93" t="s">
         <v>762</v>
       </c>
-      <c r="J25" s="52">
+      <c r="J25" s="94">
         <v>45092</v>
       </c>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52">
+      <c r="K25" s="94"/>
+      <c r="L25" s="94">
         <v>45092</v>
       </c>
-      <c r="M25" s="52"/>
-      <c r="N25" s="54" t="s">
+      <c r="M25" s="94"/>
+      <c r="N25" s="91" t="s">
         <v>783</v>
       </c>
       <c r="O25" s="54"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A26" s="72">
+      <c r="A26" s="68">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="73" t="s">
+      <c r="B26" s="70" t="s">
         <v>737</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="72" t="s">
         <v>738</v>
       </c>
       <c r="D26" s="48" t="s">
@@ -5098,12 +5272,12 @@
       <c r="O26" s="54"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A27" s="72">
+      <c r="A27" s="68">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="73"/>
-      <c r="C27" s="74"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="72"/>
       <c r="D27" s="48" t="s">
         <v>744</v>
       </c>
@@ -5130,16 +5304,16 @@
       <c r="M27" s="52">
         <v>45079</v>
       </c>
-      <c r="N27" s="56"/>
+      <c r="N27" s="55"/>
       <c r="O27" s="54"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A28" s="72">
+      <c r="A28" s="68">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="73"/>
-      <c r="C28" s="74" t="s">
+      <c r="B28" s="70"/>
+      <c r="C28" s="72" t="s">
         <v>739</v>
       </c>
       <c r="D28" s="48" t="s">
@@ -5166,12 +5340,12 @@
       <c r="O28" s="54"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A29" s="72">
+      <c r="A29" s="68">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="73"/>
-      <c r="C29" s="74"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="72"/>
       <c r="D29" s="48" t="s">
         <v>744</v>
       </c>
@@ -5204,12 +5378,12 @@
       <c r="O29" s="54"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A30" s="72">
+      <c r="A30" s="68">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="73"/>
-      <c r="C30" s="74" t="s">
+      <c r="B30" s="70"/>
+      <c r="C30" s="72" t="s">
         <v>740</v>
       </c>
       <c r="D30" s="48" t="s">
@@ -5236,12 +5410,12 @@
       <c r="O30" s="54"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A31" s="72">
+      <c r="A31" s="68">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="73"/>
-      <c r="C31" s="74"/>
+      <c r="B31" s="70"/>
+      <c r="C31" s="72"/>
       <c r="D31" s="48" t="s">
         <v>744</v>
       </c>
@@ -5274,12 +5448,12 @@
       <c r="O31" s="54"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A32" s="72">
+      <c r="A32" s="68">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="73"/>
-      <c r="C32" s="74" t="s">
+      <c r="B32" s="70"/>
+      <c r="C32" s="72" t="s">
         <v>741</v>
       </c>
       <c r="D32" s="48" t="s">
@@ -5306,23 +5480,23 @@
       <c r="O32" s="54"/>
     </row>
     <row r="33" spans="1:15" ht="24" x14ac:dyDescent="0.4">
-      <c r="A33" s="72">
+      <c r="A33" s="68">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" s="73"/>
-      <c r="C33" s="74"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="72"/>
       <c r="D33" s="48" t="s">
         <v>744</v>
       </c>
       <c r="E33" s="49"/>
       <c r="F33" s="49"/>
       <c r="G33" s="49">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H33" s="49"/>
-      <c r="I33" s="61" t="s">
-        <v>763</v>
+      <c r="I33" s="51" t="s">
+        <v>762</v>
       </c>
       <c r="J33" s="52">
         <v>45077</v>
@@ -5333,19 +5507,21 @@
       <c r="L33" s="52">
         <v>45077</v>
       </c>
-      <c r="M33" s="52"/>
-      <c r="N33" s="56" t="s">
+      <c r="M33" s="52">
+        <v>45092</v>
+      </c>
+      <c r="N33" s="55" t="s">
         <v>791</v>
       </c>
       <c r="O33" s="54"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A34" s="72">
+      <c r="A34" s="68">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" s="73"/>
-      <c r="C34" s="73" t="s">
+      <c r="B34" s="70"/>
+      <c r="C34" s="70" t="s">
         <v>742</v>
       </c>
       <c r="D34" s="48" t="s">
@@ -5368,12 +5544,12 @@
       <c r="O34" s="54"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A35" s="72">
+      <c r="A35" s="68">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B35" s="73"/>
-      <c r="C35" s="73"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="70"/>
       <c r="D35" s="48" t="s">
         <v>744</v>
       </c>
@@ -5394,11 +5570,11 @@
       <c r="O35" s="54"/>
     </row>
     <row r="36" spans="1:15" ht="60" x14ac:dyDescent="0.4">
-      <c r="A36" s="72">
+      <c r="A36" s="68">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B36" s="73"/>
+      <c r="B36" s="70"/>
       <c r="C36" s="48" t="s">
         <v>787</v>
       </c>
@@ -5406,11 +5582,11 @@
       <c r="E36" s="49"/>
       <c r="F36" s="49"/>
       <c r="G36" s="49">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H36" s="49"/>
-      <c r="I36" s="61" t="s">
-        <v>763</v>
+      <c r="I36" s="51" t="s">
+        <v>762</v>
       </c>
       <c r="J36" s="52">
         <v>45078</v>
@@ -5421,21 +5597,23 @@
       <c r="L36" s="52">
         <v>45078</v>
       </c>
-      <c r="M36" s="52"/>
-      <c r="N36" s="56" t="s">
+      <c r="M36" s="52">
+        <v>45092</v>
+      </c>
+      <c r="N36" s="55" t="s">
         <v>790</v>
       </c>
       <c r="O36" s="54"/>
     </row>
     <row r="37" spans="1:15" ht="24" x14ac:dyDescent="0.4">
-      <c r="A37" s="72">
+      <c r="A37" s="68">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B37" s="73" t="s">
+      <c r="B37" s="70" t="s">
         <v>745</v>
       </c>
-      <c r="C37" s="57" t="s">
+      <c r="C37" s="56" t="s">
         <v>749</v>
       </c>
       <c r="D37" s="48"/>
@@ -5454,18 +5632,18 @@
       <c r="K37" s="53"/>
       <c r="L37" s="52"/>
       <c r="M37" s="53"/>
-      <c r="N37" s="56" t="s">
+      <c r="N37" s="55" t="s">
         <v>789</v>
       </c>
       <c r="O37" s="54"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A38" s="72">
+      <c r="A38" s="68">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B38" s="73"/>
-      <c r="C38" s="57" t="s">
+      <c r="B38" s="70"/>
+      <c r="C38" s="56" t="s">
         <v>746</v>
       </c>
       <c r="D38" s="48"/>
@@ -5486,12 +5664,12 @@
       <c r="O38" s="54"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A39" s="72">
+      <c r="A39" s="68">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B39" s="73"/>
-      <c r="C39" s="57" t="s">
+      <c r="B39" s="70"/>
+      <c r="C39" s="56" t="s">
         <v>747</v>
       </c>
       <c r="D39" s="48"/>
@@ -5512,12 +5690,12 @@
       <c r="O39" s="54"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A40" s="72">
+      <c r="A40" s="68">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B40" s="73"/>
-      <c r="C40" s="57" t="s">
+      <c r="B40" s="70"/>
+      <c r="C40" s="56" t="s">
         <v>748</v>
       </c>
       <c r="D40" s="48"/>
@@ -5540,23 +5718,25 @@
         <v>45075</v>
       </c>
       <c r="M40" s="53"/>
-      <c r="N40" s="56" t="s">
+      <c r="N40" s="55" t="s">
         <v>775</v>
       </c>
       <c r="O40" s="54"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A41" s="72">
+      <c r="A41" s="68">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="70" t="s">
         <v>751</v>
       </c>
-      <c r="C41" s="57" t="s">
+      <c r="C41" s="56" t="s">
         <v>752</v>
       </c>
-      <c r="D41" s="48"/>
+      <c r="D41" s="48" t="s">
+        <v>805</v>
+      </c>
       <c r="E41" s="49">
         <v>100</v>
       </c>
@@ -5576,21 +5756,21 @@
         <v>45082</v>
       </c>
       <c r="M41" s="53"/>
-      <c r="N41" s="56" t="s">
+      <c r="N41" s="55" t="s">
         <v>774</v>
       </c>
       <c r="O41" s="54"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A42" s="72">
+      <c r="A42" s="68">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B42" s="73"/>
-      <c r="C42" s="57" t="s">
+      <c r="B42" s="70"/>
+      <c r="C42" s="56" t="s">
         <v>753</v>
       </c>
-      <c r="D42" s="59"/>
+      <c r="D42" s="58"/>
       <c r="E42" s="49">
         <v>100</v>
       </c>
@@ -5610,15 +5790,15 @@
       <c r="O42" s="54"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A43" s="72">
+      <c r="A43" s="68">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B43" s="73"/>
-      <c r="C43" s="57" t="s">
+      <c r="B43" s="70"/>
+      <c r="C43" s="56" t="s">
         <v>754</v>
       </c>
-      <c r="D43" s="59"/>
+      <c r="D43" s="58"/>
       <c r="E43" s="49">
         <v>100</v>
       </c>
@@ -5640,15 +5820,17 @@
       <c r="O43" s="54"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A44" s="72">
+      <c r="A44" s="68">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B44" s="73"/>
-      <c r="C44" s="57" t="s">
+      <c r="B44" s="70"/>
+      <c r="C44" s="56" t="s">
         <v>755</v>
       </c>
-      <c r="D44" s="48"/>
+      <c r="D44" s="48" t="s">
+        <v>805</v>
+      </c>
       <c r="E44" s="49">
         <v>100</v>
       </c>
@@ -5668,18 +5850,18 @@
         <v>45082</v>
       </c>
       <c r="M44" s="52"/>
-      <c r="N44" s="56" t="s">
+      <c r="N44" s="55" t="s">
         <v>773</v>
       </c>
       <c r="O44" s="54"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A45" s="72">
+      <c r="A45" s="68">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B45" s="73"/>
-      <c r="C45" s="57" t="s">
+      <c r="B45" s="70"/>
+      <c r="C45" s="56" t="s">
         <v>756</v>
       </c>
       <c r="D45" s="48"/>
@@ -5702,12 +5884,12 @@
       <c r="O45" s="54"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A46" s="72">
+      <c r="A46" s="68">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B46" s="73"/>
-      <c r="C46" s="57" t="s">
+      <c r="B46" s="70"/>
+      <c r="C46" s="56" t="s">
         <v>757</v>
       </c>
       <c r="D46" s="48"/>
@@ -5730,12 +5912,12 @@
       <c r="O46" s="54"/>
     </row>
     <row r="47" spans="1:15" ht="24" x14ac:dyDescent="0.4">
-      <c r="A47" s="72">
+      <c r="A47" s="68">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B47" s="73"/>
-      <c r="C47" s="57" t="s">
+      <c r="B47" s="70"/>
+      <c r="C47" s="56" t="s">
         <v>758</v>
       </c>
       <c r="D47" s="48"/>
@@ -5754,23 +5936,25 @@
       <c r="K47" s="52"/>
       <c r="L47" s="52"/>
       <c r="M47" s="52"/>
-      <c r="N47" s="56" t="s">
+      <c r="N47" s="55" t="s">
         <v>766</v>
       </c>
       <c r="O47" s="54"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A48" s="72">
+    <row r="48" spans="1:15" ht="48" x14ac:dyDescent="0.4">
+      <c r="A48" s="68">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B48" s="57" t="s">
+      <c r="B48" s="56" t="s">
         <v>759</v>
       </c>
-      <c r="C48" s="57" t="s">
+      <c r="C48" s="56" t="s">
         <v>760</v>
       </c>
-      <c r="D48" s="48"/>
+      <c r="D48" s="58" t="s">
+        <v>804</v>
+      </c>
       <c r="E48" s="50"/>
       <c r="F48" s="50"/>
       <c r="G48" s="49">
@@ -5785,26 +5969,28 @@
       </c>
       <c r="K48" s="52"/>
       <c r="L48" s="52">
-        <v>45083</v>
+        <v>45105</v>
       </c>
       <c r="M48" s="53"/>
-      <c r="N48" s="56" t="s">
+      <c r="N48" s="55" t="s">
         <v>761</v>
       </c>
       <c r="O48" s="54"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A49" s="72">
+    <row r="49" spans="1:15" ht="24" x14ac:dyDescent="0.4">
+      <c r="A49" s="68">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B49" s="75" t="s">
+      <c r="B49" s="69" t="s">
         <v>779</v>
       </c>
-      <c r="C49" s="57" t="s">
+      <c r="C49" s="56" t="s">
         <v>776</v>
       </c>
-      <c r="D49" s="48"/>
+      <c r="D49" s="58" t="s">
+        <v>803</v>
+      </c>
       <c r="E49" s="49"/>
       <c r="F49" s="49"/>
       <c r="G49" s="49"/>
@@ -5813,31 +5999,29 @@
         <v>762</v>
       </c>
       <c r="J49" s="52">
-        <v>45076</v>
+        <v>45100</v>
       </c>
       <c r="K49" s="52"/>
       <c r="L49" s="52">
-        <v>45086</v>
+        <v>45103</v>
       </c>
       <c r="M49" s="53"/>
       <c r="N49" s="54"/>
       <c r="O49" s="54"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A50" s="72">
+    <row r="50" spans="1:15" ht="24" x14ac:dyDescent="0.4">
+      <c r="A50" s="68">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B50" s="75"/>
+      <c r="B50" s="69"/>
       <c r="C50" s="57" t="s">
         <v>780</v>
       </c>
       <c r="D50" s="48"/>
       <c r="E50" s="49"/>
       <c r="F50" s="49"/>
-      <c r="G50" s="49">
-        <v>20</v>
-      </c>
+      <c r="G50" s="49"/>
       <c r="H50" s="49"/>
       <c r="I50" s="51" t="s">
         <v>762</v>
@@ -5850,18 +6034,18 @@
         <v>45086</v>
       </c>
       <c r="M50" s="53"/>
-      <c r="N50" s="56"/>
+      <c r="N50" s="55"/>
       <c r="O50" s="54"/>
     </row>
     <row r="51" spans="1:15" ht="24" x14ac:dyDescent="0.4">
-      <c r="A51" s="72">
+      <c r="A51" s="68">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B51" s="58" t="s">
+      <c r="B51" s="57" t="s">
         <v>778</v>
       </c>
-      <c r="C51" s="57"/>
+      <c r="C51" s="56"/>
       <c r="D51" s="48"/>
       <c r="E51" s="49"/>
       <c r="F51" s="49"/>
@@ -5869,8 +6053,8 @@
         <v>100</v>
       </c>
       <c r="H51" s="49"/>
-      <c r="I51" s="61" t="s">
-        <v>763</v>
+      <c r="I51" s="51" t="s">
+        <v>764</v>
       </c>
       <c r="J51" s="52">
         <v>45077</v>
@@ -5884,178 +6068,262 @@
       <c r="M51" s="52">
         <v>45077</v>
       </c>
-      <c r="N51" s="56" t="s">
+      <c r="N51" s="55" t="s">
         <v>777</v>
       </c>
       <c r="O51" s="54"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A52" s="72">
+      <c r="A52" s="68">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B52" s="57"/>
-      <c r="C52" s="57"/>
+      <c r="B52" s="56" t="s">
+        <v>792</v>
+      </c>
+      <c r="C52" s="56"/>
       <c r="D52" s="48"/>
       <c r="E52" s="49"/>
       <c r="F52" s="49"/>
       <c r="G52" s="49"/>
       <c r="H52" s="49"/>
-      <c r="I52" s="51"/>
-      <c r="J52" s="52"/>
+      <c r="I52" s="100" t="s">
+        <v>763</v>
+      </c>
+      <c r="J52" s="52">
+        <v>45098</v>
+      </c>
       <c r="K52" s="52"/>
-      <c r="L52" s="52"/>
+      <c r="L52" s="52">
+        <v>45099</v>
+      </c>
       <c r="M52" s="53"/>
       <c r="N52" s="54"/>
       <c r="O52" s="54"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B53" s="66"/>
-      <c r="C53" s="66"/>
-      <c r="D53" s="62"/>
-      <c r="E53" s="67"/>
-      <c r="F53" s="67"/>
-      <c r="G53" s="67"/>
-      <c r="H53" s="67"/>
-      <c r="I53" s="68"/>
-      <c r="J53" s="69"/>
-      <c r="K53" s="69"/>
-      <c r="L53" s="69"/>
-      <c r="M53" s="70"/>
-      <c r="N53" s="71"/>
-      <c r="O53" s="71"/>
+      <c r="B53" s="96" t="s">
+        <v>793</v>
+      </c>
+      <c r="C53" s="64" t="s">
+        <v>795</v>
+      </c>
+      <c r="D53" s="60"/>
+      <c r="E53" s="65"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="65"/>
+      <c r="H53" s="65"/>
+      <c r="I53" s="51" t="s">
+        <v>762</v>
+      </c>
+      <c r="J53" s="52">
+        <v>45097</v>
+      </c>
+      <c r="K53" s="53"/>
+      <c r="L53" s="52">
+        <v>45106</v>
+      </c>
+      <c r="M53" s="66"/>
+      <c r="N53" s="67"/>
+      <c r="O53" s="67"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B54" s="57"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="48"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="49"/>
-      <c r="G54" s="49"/>
-      <c r="H54" s="49"/>
-      <c r="I54" s="51"/>
-      <c r="J54" s="52"/>
-      <c r="K54" s="52"/>
-      <c r="L54" s="52"/>
-      <c r="M54" s="53"/>
-      <c r="N54" s="54"/>
-      <c r="O54" s="54"/>
+      <c r="B54" s="97"/>
+      <c r="C54" s="64" t="s">
+        <v>796</v>
+      </c>
+      <c r="D54" s="60"/>
+      <c r="E54" s="65"/>
+      <c r="F54" s="65"/>
+      <c r="G54" s="65"/>
+      <c r="H54" s="65"/>
+      <c r="I54" s="51" t="s">
+        <v>762</v>
+      </c>
+      <c r="J54" s="52">
+        <v>45097</v>
+      </c>
+      <c r="K54" s="53"/>
+      <c r="L54" s="52">
+        <v>45106</v>
+      </c>
+      <c r="M54" s="66"/>
+      <c r="N54" s="67"/>
+      <c r="O54" s="67"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B55" s="57"/>
-      <c r="C55" s="57"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="49"/>
-      <c r="F55" s="49"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="49"/>
-      <c r="I55" s="51"/>
-      <c r="J55" s="52"/>
-      <c r="K55" s="52"/>
-      <c r="L55" s="52"/>
-      <c r="M55" s="53"/>
-      <c r="N55" s="54"/>
-      <c r="O55" s="54"/>
+      <c r="B55" s="97"/>
+      <c r="C55" s="64" t="s">
+        <v>797</v>
+      </c>
+      <c r="D55" s="60"/>
+      <c r="E55" s="65"/>
+      <c r="F55" s="65"/>
+      <c r="G55" s="65"/>
+      <c r="H55" s="65"/>
+      <c r="I55" s="51" t="s">
+        <v>762</v>
+      </c>
+      <c r="J55" s="52">
+        <v>45097</v>
+      </c>
+      <c r="K55" s="53"/>
+      <c r="L55" s="52">
+        <v>45106</v>
+      </c>
+      <c r="M55" s="66"/>
+      <c r="N55" s="67"/>
+      <c r="O55" s="67"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B56" s="57"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="48"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="49"/>
-      <c r="G56" s="49"/>
-      <c r="H56" s="49"/>
-      <c r="I56" s="51"/>
-      <c r="J56" s="52"/>
-      <c r="K56" s="52"/>
-      <c r="L56" s="52"/>
-      <c r="M56" s="53"/>
-      <c r="N56" s="54"/>
-      <c r="O56" s="54"/>
+      <c r="B56" s="97"/>
+      <c r="C56" s="64" t="s">
+        <v>798</v>
+      </c>
+      <c r="D56" s="60"/>
+      <c r="E56" s="65"/>
+      <c r="F56" s="65"/>
+      <c r="G56" s="65"/>
+      <c r="H56" s="65"/>
+      <c r="I56" s="51" t="s">
+        <v>762</v>
+      </c>
+      <c r="J56" s="52">
+        <v>45097</v>
+      </c>
+      <c r="K56" s="53"/>
+      <c r="L56" s="52">
+        <v>45106</v>
+      </c>
+      <c r="M56" s="66"/>
+      <c r="N56" s="67"/>
+      <c r="O56" s="67"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B57" s="57"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="59"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="49"/>
-      <c r="I57" s="51"/>
-      <c r="J57" s="52"/>
-      <c r="K57" s="52"/>
-      <c r="L57" s="52"/>
-      <c r="M57" s="53"/>
-      <c r="N57" s="54"/>
-      <c r="O57" s="54"/>
+      <c r="B57" s="97"/>
+      <c r="C57" s="64" t="s">
+        <v>799</v>
+      </c>
+      <c r="D57" s="60"/>
+      <c r="E57" s="65"/>
+      <c r="F57" s="65"/>
+      <c r="G57" s="65"/>
+      <c r="H57" s="65"/>
+      <c r="I57" s="51" t="s">
+        <v>762</v>
+      </c>
+      <c r="J57" s="52">
+        <v>45097</v>
+      </c>
+      <c r="K57" s="53"/>
+      <c r="L57" s="52">
+        <v>45106</v>
+      </c>
+      <c r="M57" s="66"/>
+      <c r="N57" s="67"/>
+      <c r="O57" s="67"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B58" s="57"/>
-      <c r="C58" s="57"/>
-      <c r="D58" s="48"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="49"/>
-      <c r="I58" s="51"/>
-      <c r="J58" s="52"/>
-      <c r="K58" s="52"/>
-      <c r="L58" s="52"/>
-      <c r="M58" s="53"/>
-      <c r="N58" s="54"/>
-      <c r="O58" s="54"/>
+      <c r="B58" s="97"/>
+      <c r="C58" s="64" t="s">
+        <v>800</v>
+      </c>
+      <c r="D58" s="60"/>
+      <c r="E58" s="65"/>
+      <c r="F58" s="65"/>
+      <c r="G58" s="65"/>
+      <c r="H58" s="65"/>
+      <c r="I58" s="51" t="s">
+        <v>762</v>
+      </c>
+      <c r="J58" s="52">
+        <v>45097</v>
+      </c>
+      <c r="K58" s="53"/>
+      <c r="L58" s="52">
+        <v>45106</v>
+      </c>
+      <c r="M58" s="66"/>
+      <c r="N58" s="67"/>
+      <c r="O58" s="67"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B59" s="57"/>
-      <c r="C59" s="57"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="49"/>
-      <c r="I59" s="51"/>
-      <c r="J59" s="52"/>
-      <c r="K59" s="52"/>
-      <c r="L59" s="52"/>
-      <c r="M59" s="53"/>
-      <c r="N59" s="54"/>
-      <c r="O59" s="54"/>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B60" s="57"/>
-      <c r="C60" s="57"/>
+      <c r="B59" s="98"/>
+      <c r="C59" s="64" t="s">
+        <v>801</v>
+      </c>
+      <c r="D59" s="60"/>
+      <c r="E59" s="65"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="65"/>
+      <c r="H59" s="65"/>
+      <c r="I59" s="51" t="s">
+        <v>762</v>
+      </c>
+      <c r="J59" s="52">
+        <v>45097</v>
+      </c>
+      <c r="K59" s="53"/>
+      <c r="L59" s="52">
+        <v>45106</v>
+      </c>
+      <c r="M59" s="66"/>
+      <c r="N59" s="67"/>
+      <c r="O59" s="67"/>
+    </row>
+    <row r="60" spans="1:15" ht="24" x14ac:dyDescent="0.4">
+      <c r="B60" s="56" t="s">
+        <v>794</v>
+      </c>
+      <c r="C60" s="56"/>
       <c r="D60" s="48"/>
       <c r="E60" s="49"/>
       <c r="F60" s="49"/>
       <c r="G60" s="49"/>
       <c r="H60" s="49"/>
-      <c r="I60" s="51"/>
-      <c r="J60" s="52"/>
-      <c r="K60" s="52"/>
-      <c r="L60" s="52"/>
+      <c r="I60" s="100" t="s">
+        <v>763</v>
+      </c>
+      <c r="J60" s="52">
+        <v>45100</v>
+      </c>
+      <c r="K60" s="53"/>
+      <c r="L60" s="52">
+        <v>45100</v>
+      </c>
       <c r="M60" s="53"/>
-      <c r="N60" s="54"/>
+      <c r="N60" s="55" t="s">
+        <v>806</v>
+      </c>
       <c r="O60" s="54"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B61" s="57"/>
-      <c r="C61" s="57"/>
+      <c r="B61" s="56" t="s">
+        <v>802</v>
+      </c>
+      <c r="C61" s="56"/>
       <c r="D61" s="48"/>
       <c r="E61" s="49"/>
       <c r="F61" s="49"/>
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
-      <c r="I61" s="51"/>
-      <c r="J61" s="52"/>
-      <c r="K61" s="52"/>
-      <c r="L61" s="52"/>
+      <c r="I61" s="100" t="s">
+        <v>763</v>
+      </c>
+      <c r="J61" s="52">
+        <v>45100</v>
+      </c>
+      <c r="K61" s="53"/>
+      <c r="L61" s="52">
+        <v>45100</v>
+      </c>
       <c r="M61" s="53"/>
       <c r="N61" s="54"/>
       <c r="O61" s="54"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B62" s="57"/>
-      <c r="C62" s="57"/>
+      <c r="B62" s="56"/>
+      <c r="C62" s="56"/>
       <c r="D62" s="48"/>
       <c r="E62" s="49"/>
       <c r="F62" s="49"/>
@@ -6070,9 +6338,9 @@
       <c r="O62" s="54"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B63" s="57"/>
-      <c r="C63" s="57"/>
-      <c r="D63" s="48"/>
+      <c r="B63" s="56"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="58"/>
       <c r="E63" s="49"/>
       <c r="F63" s="49"/>
       <c r="G63" s="49"/>
@@ -6085,9 +6353,116 @@
       <c r="N63" s="54"/>
       <c r="O63" s="54"/>
     </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B64" s="56"/>
+      <c r="C64" s="56"/>
+      <c r="D64" s="48"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="51"/>
+      <c r="J64" s="52"/>
+      <c r="K64" s="52"/>
+      <c r="L64" s="52"/>
+      <c r="M64" s="53"/>
+      <c r="N64" s="54"/>
+      <c r="O64" s="54"/>
+    </row>
+    <row r="65" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B65" s="56"/>
+      <c r="C65" s="56"/>
+      <c r="D65" s="48"/>
+      <c r="E65" s="49"/>
+      <c r="F65" s="49"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="49"/>
+      <c r="I65" s="51"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="52"/>
+      <c r="L65" s="52"/>
+      <c r="M65" s="53"/>
+      <c r="N65" s="54"/>
+      <c r="O65" s="54"/>
+    </row>
+    <row r="66" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B66" s="56"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="48"/>
+      <c r="E66" s="49"/>
+      <c r="F66" s="49"/>
+      <c r="G66" s="49"/>
+      <c r="H66" s="49"/>
+      <c r="I66" s="51"/>
+      <c r="J66" s="52"/>
+      <c r="K66" s="52"/>
+      <c r="L66" s="52"/>
+      <c r="M66" s="53"/>
+      <c r="N66" s="54"/>
+      <c r="O66" s="54"/>
+    </row>
+    <row r="67" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B67" s="56"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="48"/>
+      <c r="E67" s="49"/>
+      <c r="F67" s="49"/>
+      <c r="G67" s="49"/>
+      <c r="H67" s="49"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="52"/>
+      <c r="K67" s="52"/>
+      <c r="L67" s="52"/>
+      <c r="M67" s="53"/>
+      <c r="N67" s="54"/>
+      <c r="O67" s="54"/>
+    </row>
+    <row r="68" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B68" s="56"/>
+      <c r="C68" s="56"/>
+      <c r="D68" s="48"/>
+      <c r="E68" s="49"/>
+      <c r="F68" s="49"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="49"/>
+      <c r="I68" s="51"/>
+      <c r="J68" s="52"/>
+      <c r="K68" s="52"/>
+      <c r="L68" s="52"/>
+      <c r="M68" s="53"/>
+      <c r="N68" s="54"/>
+      <c r="O68" s="54"/>
+    </row>
+    <row r="69" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B69" s="56"/>
+      <c r="C69" s="56"/>
+      <c r="D69" s="48"/>
+      <c r="E69" s="49"/>
+      <c r="F69" s="49"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="49"/>
+      <c r="I69" s="51"/>
+      <c r="J69" s="52"/>
+      <c r="K69" s="52"/>
+      <c r="L69" s="52"/>
+      <c r="M69" s="53"/>
+      <c r="N69" s="54"/>
+      <c r="O69" s="54"/>
+    </row>
   </sheetData>
   <autoFilter ref="B1:O51" xr:uid="{8E7929DC-B531-419A-8BB3-4B492C6A9455}"/>
-  <mergeCells count="22">
+  <mergeCells count="23">
+    <mergeCell ref="B53:B59"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B26:B36"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B2:B14"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B15:B19"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="B41:B47"/>
     <mergeCell ref="E15:H15"/>
@@ -6100,45 +6475,46 @@
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="E18:H18"/>
     <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B26:B36"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B2:B14"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B15:B19"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="J2:J63">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>$J2=TODAY()</formula>
+  <conditionalFormatting sqref="J2:J69">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>$J2=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>$J2&lt;TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>$J2=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L63">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$J2=""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$J2&lt;TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>$J2=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L15 L18:L69">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$J2=""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>$J2&lt;TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>$J2=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L16:L17">
+    <cfRule type="expression" dxfId="8" priority="1">
+      <formula>$J16=""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="2">
+      <formula>$J16&lt;TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>$J16=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:H14 E2:E63 F21:H63" xr:uid="{AE3AF69A-B4F7-4B81-A2BD-52A1686AE65E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:H14 F21:H69 E2:E69" xr:uid="{AE3AF69A-B4F7-4B81-A2BD-52A1686AE65E}">
       <formula1>"20, 40, 60, 80, 100"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I63" xr:uid="{A42C63AA-A747-4737-B92C-155730460CEA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I69" xr:uid="{A42C63AA-A747-4737-B92C-155730460CEA}">
       <formula1>"Low, Medium, High"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6216,7 +6592,7 @@
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="79" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -6240,7 +6616,7 @@
       <c r="O3" s="14"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B4" s="81"/>
+      <c r="B4" s="80"/>
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
@@ -6266,7 +6642,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B5" s="81"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
@@ -6292,7 +6668,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B6" s="81"/>
+      <c r="B6" s="80"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
@@ -6318,7 +6694,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B7" s="81"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
@@ -6340,7 +6716,7 @@
       <c r="O7" s="14"/>
     </row>
     <row r="8" spans="2:18" ht="93" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="82"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
@@ -6372,7 +6748,7 @@
       <c r="O8" s="14"/>
     </row>
     <row r="9" spans="2:18" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="79" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -6406,7 +6782,7 @@
       <c r="O9" s="14"/>
     </row>
     <row r="10" spans="2:18" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="B10" s="81"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="1" t="s">
         <v>62</v>
       </c>
@@ -6438,7 +6814,7 @@
       <c r="O10" s="14"/>
     </row>
     <row r="11" spans="2:18" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="82" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -6472,7 +6848,7 @@
       <c r="O11" s="14"/>
     </row>
     <row r="12" spans="2:18" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="B12" s="92"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="1" t="s">
         <v>17</v>
       </c>
@@ -6504,7 +6880,7 @@
       <c r="O12" s="14"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B13" s="92"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
@@ -6534,7 +6910,7 @@
       <c r="O13" s="14"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="79" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -6566,7 +6942,7 @@
       <c r="O14" s="14"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B15" s="81"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="1" t="s">
         <v>66</v>
       </c>
@@ -6596,7 +6972,7 @@
       <c r="O15" s="14"/>
     </row>
     <row r="16" spans="2:18" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="81"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
@@ -6628,7 +7004,7 @@
       </c>
     </row>
     <row r="17" spans="2:15" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="B17" s="81"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
@@ -6660,8 +7036,8 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B18" s="81"/>
-      <c r="C18" s="83" t="s">
+      <c r="B18" s="80"/>
+      <c r="C18" s="73" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="14" t="s">
@@ -6692,8 +7068,8 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B19" s="81"/>
-      <c r="C19" s="85"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="74"/>
       <c r="D19" s="14" t="s">
         <v>47</v>
       </c>
@@ -6722,8 +7098,8 @@
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B20" s="81"/>
-      <c r="C20" s="85"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="74"/>
       <c r="D20" s="14" t="s">
         <v>48</v>
       </c>
@@ -6752,8 +7128,8 @@
       <c r="O20" s="14"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B21" s="81"/>
-      <c r="C21" s="85"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="74"/>
       <c r="D21" s="14" t="s">
         <v>49</v>
       </c>
@@ -6782,8 +7158,8 @@
       <c r="O21" s="14"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B22" s="81"/>
-      <c r="C22" s="85"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="74"/>
       <c r="D22" s="22" t="s">
         <v>50</v>
       </c>
@@ -6812,8 +7188,8 @@
       <c r="O22" s="14"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B23" s="81"/>
-      <c r="C23" s="85"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="74"/>
       <c r="D23" s="14" t="s">
         <v>51</v>
       </c>
@@ -6842,8 +7218,8 @@
       <c r="O23" s="14"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B24" s="81"/>
-      <c r="C24" s="85"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="74"/>
       <c r="D24" s="14" t="s">
         <v>52</v>
       </c>
@@ -6872,8 +7248,8 @@
       <c r="O24" s="14"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B25" s="81"/>
-      <c r="C25" s="84"/>
+      <c r="B25" s="80"/>
+      <c r="C25" s="75"/>
       <c r="D25" s="14" t="s">
         <v>53</v>
       </c>
@@ -6902,7 +7278,7 @@
       <c r="O25" s="14"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B26" s="80" t="s">
+      <c r="B26" s="79" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -6928,7 +7304,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B27" s="81"/>
+      <c r="B27" s="80"/>
       <c r="C27" s="1" t="s">
         <v>28</v>
       </c>
@@ -6952,7 +7328,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B28" s="80" t="s">
+      <c r="B28" s="79" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -6982,7 +7358,7 @@
       <c r="O28" s="14"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B29" s="81"/>
+      <c r="B29" s="80"/>
       <c r="C29" s="1" t="s">
         <v>43</v>
       </c>
@@ -7010,8 +7386,8 @@
       <c r="O29" s="14"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B30" s="81"/>
-      <c r="C30" s="83" t="s">
+      <c r="B30" s="80"/>
+      <c r="C30" s="73" t="s">
         <v>44</v>
       </c>
       <c r="D30" s="14" t="s">
@@ -7040,8 +7416,8 @@
       <c r="O30" s="14"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B31" s="81"/>
-      <c r="C31" s="85"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="74"/>
       <c r="D31" s="14"/>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -7056,8 +7432,8 @@
       <c r="O31" s="14"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B32" s="82"/>
-      <c r="C32" s="84"/>
+      <c r="B32" s="81"/>
+      <c r="C32" s="75"/>
       <c r="D32" s="14"/>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
@@ -7072,7 +7448,7 @@
       <c r="O32" s="14"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B33" s="80" t="s">
+      <c r="B33" s="79" t="s">
         <v>24</v>
       </c>
       <c r="C33" s="14" t="s">
@@ -7098,7 +7474,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B34" s="81"/>
+      <c r="B34" s="80"/>
       <c r="C34" s="14" t="s">
         <v>39</v>
       </c>
@@ -7122,7 +7498,7 @@
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B35" s="81"/>
+      <c r="B35" s="80"/>
       <c r="C35" s="14" t="s">
         <v>40</v>
       </c>
@@ -7146,8 +7522,8 @@
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B36" s="81"/>
-      <c r="C36" s="88" t="s">
+      <c r="B36" s="80"/>
+      <c r="C36" s="76" t="s">
         <v>41</v>
       </c>
       <c r="D36" s="14"/>
@@ -7170,8 +7546,8 @@
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B37" s="81"/>
-      <c r="C37" s="89"/>
+      <c r="B37" s="80"/>
+      <c r="C37" s="77"/>
       <c r="D37" s="14"/>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
@@ -7192,8 +7568,8 @@
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B38" s="82"/>
-      <c r="C38" s="90"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="78"/>
       <c r="D38" s="14"/>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
@@ -7282,10 +7658,10 @@
       <c r="O41" s="10"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B42" s="80" t="s">
+      <c r="B42" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="77" t="s">
+      <c r="C42" s="84" t="s">
         <v>30</v>
       </c>
       <c r="D42" s="14" t="s">
@@ -7316,8 +7692,8 @@
       <c r="O42" s="14"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B43" s="81"/>
-      <c r="C43" s="79"/>
+      <c r="B43" s="80"/>
+      <c r="C43" s="86"/>
       <c r="D43" s="14" t="s">
         <v>31</v>
       </c>
@@ -7346,8 +7722,8 @@
       <c r="O43" s="14"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B44" s="81"/>
-      <c r="C44" s="83"/>
+      <c r="B44" s="80"/>
+      <c r="C44" s="73"/>
       <c r="D44" s="14" t="s">
         <v>34</v>
       </c>
@@ -7376,8 +7752,8 @@
       <c r="O44" s="14"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B45" s="82"/>
-      <c r="C45" s="84"/>
+      <c r="B45" s="81"/>
+      <c r="C45" s="75"/>
       <c r="D45" s="14" t="s">
         <v>31</v>
       </c>
@@ -7406,7 +7782,7 @@
       <c r="O45" s="14"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B46" s="80" t="s">
+      <c r="B46" s="79" t="s">
         <v>74</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -7428,7 +7804,7 @@
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B47" s="81"/>
+      <c r="B47" s="80"/>
       <c r="C47" s="1" t="s">
         <v>76</v>
       </c>
@@ -7448,7 +7824,7 @@
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B48" s="81"/>
+      <c r="B48" s="80"/>
       <c r="C48" s="1" t="s">
         <v>77</v>
       </c>
@@ -7468,7 +7844,7 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B49" s="81"/>
+      <c r="B49" s="80"/>
       <c r="C49" s="1" t="s">
         <v>78</v>
       </c>
@@ -7488,7 +7864,7 @@
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B50" s="82"/>
+      <c r="B50" s="81"/>
       <c r="C50" s="1" t="s">
         <v>79</v>
       </c>
@@ -7508,10 +7884,10 @@
       </c>
     </row>
     <row r="51" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="80" t="s">
+      <c r="B51" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="77" t="s">
+      <c r="C51" s="84" t="s">
         <v>84</v>
       </c>
       <c r="D51" s="14" t="s">
@@ -7532,8 +7908,8 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B52" s="81"/>
-      <c r="C52" s="78"/>
+      <c r="B52" s="80"/>
+      <c r="C52" s="85"/>
       <c r="D52" s="14" t="s">
         <v>86</v>
       </c>
@@ -7552,8 +7928,8 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B53" s="82"/>
-      <c r="C53" s="79"/>
+      <c r="B53" s="81"/>
+      <c r="C53" s="86"/>
       <c r="D53" s="14" t="s">
         <v>87</v>
       </c>
@@ -7637,7 +8013,7 @@
     </row>
     <row r="57" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B57" s="6"/>
-      <c r="C57" s="86" t="s">
+      <c r="C57" s="87" t="s">
         <v>93</v>
       </c>
       <c r="D57" s="14" t="s">
@@ -7659,7 +8035,7 @@
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B58" s="6"/>
-      <c r="C58" s="87"/>
+      <c r="C58" s="88"/>
       <c r="D58" s="14" t="s">
         <v>95</v>
       </c>
@@ -8085,7 +8461,7 @@
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B80" s="6"/>
-      <c r="C80" s="83" t="s">
+      <c r="C80" s="73" t="s">
         <v>114</v>
       </c>
       <c r="D80" s="14" t="s">
@@ -8107,7 +8483,7 @@
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B81" s="6"/>
-      <c r="C81" s="85"/>
+      <c r="C81" s="74"/>
       <c r="D81" s="14" t="s">
         <v>95</v>
       </c>
@@ -8127,7 +8503,7 @@
     </row>
     <row r="82" spans="2:15" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B82" s="6"/>
-      <c r="C82" s="84"/>
+      <c r="C82" s="75"/>
       <c r="D82" s="21" t="s">
         <v>115</v>
       </c>
@@ -8265,7 +8641,7 @@
     </row>
     <row r="89" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B89" s="6"/>
-      <c r="C89" s="77" t="s">
+      <c r="C89" s="84" t="s">
         <v>133</v>
       </c>
       <c r="D89" s="24" t="s">
@@ -8287,7 +8663,7 @@
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B90" s="6"/>
-      <c r="C90" s="78"/>
+      <c r="C90" s="85"/>
       <c r="D90" s="24" t="s">
         <v>136</v>
       </c>
@@ -8307,7 +8683,7 @@
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B91" s="6"/>
-      <c r="C91" s="78"/>
+      <c r="C91" s="85"/>
       <c r="D91" s="24" t="s">
         <v>135</v>
       </c>
@@ -8327,7 +8703,7 @@
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B92" s="6"/>
-      <c r="C92" s="79"/>
+      <c r="C92" s="86"/>
       <c r="D92" s="28" t="s">
         <v>137</v>
       </c>
@@ -8586,6 +8962,15 @@
   </sheetData>
   <autoFilter ref="I2:I47" xr:uid="{6EBC6241-952D-451D-ACB1-930264AC8260}"/>
   <mergeCells count="19">
+    <mergeCell ref="C89:C92"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="C57:C58"/>
     <mergeCell ref="C18:C25"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="C36:C38"/>
@@ -8596,15 +8981,6 @@
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="B33:B38"/>
-    <mergeCell ref="C89:C92"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C80:C82"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="C57:C58"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>